<commit_message>
Homepage revisions and clean up
</commit_message>
<xml_diff>
--- a/tasklist.xlsx
+++ b/tasklist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -46,9 +46,6 @@
     <t>randomize initial image in rotator on page refresh</t>
   </si>
   <si>
-    <t>add SCROLL prompts at the bottom edge of the screen that disappears when scrolled</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>*header</t>
   </si>
   <si>
-    <t>when main nav collides with logo (at around 1024 wide), switch to hamburger menu</t>
-  </si>
-  <si>
     <t>Layout</t>
   </si>
   <si>
@@ -88,30 +82,15 @@
     <t>Get TOS/PP from legal</t>
   </si>
   <si>
-    <t>change copyright from Six Foot, LCC to just Six Foot</t>
-  </si>
-  <si>
     <t>art</t>
   </si>
   <si>
     <t>select hero imagery</t>
   </si>
   <si>
-    <t>on business unit buttons display identifier. (e.g. GAMES)</t>
-  </si>
-  <si>
     <t>select imagery for business unit buttons (based on subsection hero imagery)</t>
   </si>
   <si>
-    <t>Revise copy for: We build experiences and products for people and provide professional services for businesses.</t>
-  </si>
-  <si>
-    <t>Place revised copy on homepage (based on revisions)</t>
-  </si>
-  <si>
-    <t>add current clients (Grey Box, Marvel?, Magic Leap, etc)</t>
-  </si>
-  <si>
     <t>Pictures</t>
   </si>
   <si>
@@ -149,6 +128,30 @@
   </si>
   <si>
     <t>include staffing client logos</t>
+  </si>
+  <si>
+    <t>Revise homepage copy.</t>
+  </si>
+  <si>
+    <t>between widths 768 and 1035, the main nav breaks the layout - this can impact the logo carousel.</t>
+  </si>
+  <si>
+    <t>the sticky header bounces when it transitions</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>images need to be optimized - target: 4k resolution where possible; compression high (8).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have mobile sites load appropriately sized images </t>
+  </si>
+  <si>
+    <t>implement Google Analytic (basic page views)</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -531,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -540,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -557,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -565,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -574,168 +577,168 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -744,242 +747,242 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
@@ -987,45 +990,31 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B95:B102 A2:A102">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90:B97 A72:A97">
       <formula1>"Home,Games,Pictures,Press,Adventures,Promo,Staffing,Agency,Technology,Capital,Contact,Careers,Our Story, *header,*footer,*metadata"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C109">
       <formula1>"art,copy,programming,design"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A71">
+      <formula1>"Home,Games,Pictures,Press,Adventures,Promo,Staffing,Agency,Technology,Capital,Contact,Careers,Our Story, Global, *header,*footer,*metadata"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>